<commit_message>
debugging system, now sysA matches results from Trimmer et al.
</commit_message>
<xml_diff>
--- a/qsdsan/systems/bwaise/results/lca_report.xlsx
+++ b/qsdsan/systems/bwaise/results/lca_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/qs_yl/qsdsan/systems/bwaise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_AF7EC33461C80B9C38379B1CBAEF6DAB61B4ED88" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28B6F807-1B21-0346-A8FA-86391F79DBF2}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_AF7EC3345AB88D6F3F64A79E60AC774160B4E23B" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3FB9D626-BCA4-0345-91B1-4A6E6AC4B422}"/>
   <bookViews>
-    <workbookView xWindow="17360" yWindow="1340" windowWidth="21040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26440" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>GlobalWarming [kg CO2-eq]</t>
   </si>
   <si>
-    <t>Total GlobalWarming Ratio</t>
+    <t>Category GlobalWarming Ratio</t>
   </si>
   <si>
     <t>Construction</t>
@@ -87,18 +87,18 @@
     <t>Total</t>
   </si>
   <si>
-    <t>A4</t>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A6</t>
   </si>
   <si>
     <t>A7</t>
   </si>
   <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -114,7 +114,7 @@
     <t>Mass [kg]</t>
   </si>
   <si>
-    <t>WasteStream</t>
+    <t>Stream</t>
   </si>
   <si>
     <t>fugitive_CH4</t>
@@ -549,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,12 +560,12 @@
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -593,45 +593,37 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>567000</v>
+        <v>5906254.7249999996</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>158760</v>
+        <v>1653751.3230000001</v>
       </c>
       <c r="F2">
-        <v>3.3564519070733913E-2</v>
-      </c>
-      <c r="H2">
-        <f>E2/40000/8</f>
-        <v>0.49612499999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5.7460786610612852E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>567000</v>
+        <v>5906254.7249999996</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>158760</v>
+        <v>1653751.3230000001</v>
       </c>
       <c r="F3">
-        <v>3.3564519070733913E-2</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H27" si="0">E3/40000/8</f>
-        <v>0.49612499999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5.7460786610612852E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -639,45 +631,37 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>1750000</v>
+        <v>18229181.25</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1890000</v>
+        <v>19687515.75</v>
       </c>
       <c r="F4">
-        <v>0.39957760798492747</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>5.90625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.6840569834596768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>1750000</v>
+        <v>18229181.25</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1890000</v>
+        <v>19687515.75</v>
       </c>
       <c r="F5">
-        <v>0.39957760798492747</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>5.90625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.6840569834596768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -694,14 +678,10 @@
         <v>129913.3497553824</v>
       </c>
       <c r="F6">
-        <v>2.7465854783367692E-2</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>0.40597921798557002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4.5139333612880441E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -716,14 +696,10 @@
         <v>1817442</v>
       </c>
       <c r="F7">
-        <v>0.38423763333933458</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>5.6795062500000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6.3148337653160816E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
@@ -738,14 +714,10 @@
         <v>1947355.3497553819</v>
       </c>
       <c r="F8">
-        <v>0.4117034881227023</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>6.0854854679855688</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6.7662271014448869E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -753,23 +725,19 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>9140.0000000000018</v>
+        <v>95208.409500000009</v>
       </c>
       <c r="D9">
-        <v>0.19213300792532439</v>
+        <v>0.7124265141203362</v>
       </c>
       <c r="E9">
-        <v>4844.2000000000016</v>
+        <v>50460.457035000007</v>
       </c>
       <c r="F9">
-        <v>1.024144893439464E-3</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>1.5138125000000006E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.7532851001456969E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
@@ -778,20 +746,16 @@
         <v>1451.211728244062</v>
       </c>
       <c r="D10">
-        <v>3.050609130022321E-2</v>
+        <v>1.0859142781956309E-2</v>
       </c>
       <c r="E10">
         <v>769.14221596935306</v>
       </c>
       <c r="F10">
-        <v>1.62609527437704E-4</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>2.4035694249042285E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.6724402956096018E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -800,20 +764,16 @@
         <v>13920</v>
       </c>
       <c r="D11">
-        <v>0.29261394642456412</v>
+        <v>0.1041607262282339</v>
       </c>
       <c r="E11">
         <v>7377.6</v>
       </c>
       <c r="F11">
-        <v>1.559748021518307E-3</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>2.3055000000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.5634005149543121E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -822,42 +782,34 @@
         <v>23060</v>
       </c>
       <c r="D12">
-        <v>0.4847469543498884</v>
+        <v>0.1725536168694736</v>
       </c>
       <c r="E12">
         <v>12221.8</v>
       </c>
       <c r="F12">
-        <v>2.583892914957771E-3</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>3.8193124999999994E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4.2465528645723003E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13">
-        <v>47571.211728244059</v>
+        <v>133639.6212282441</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>25212.742215969349</v>
+        <v>70828.999250969355</v>
       </c>
       <c r="F13">
-        <v>5.330395357353245E-3</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>7.878981942490422E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.4610048410544541E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -865,45 +817,37 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>3200000</v>
+        <v>33333360</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>48000</v>
+        <v>500000.4</v>
       </c>
       <c r="F14">
-        <v>1.0148002742474351E-2</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.737287577040449E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15">
-        <v>3200000</v>
+        <v>33333360</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>48000</v>
+        <v>500000.4</v>
       </c>
       <c r="F15">
-        <v>1.0148002742474351E-2</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.737287577040449E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -911,23 +855,19 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>25200</v>
+        <v>262500.21000000002</v>
       </c>
       <c r="D16">
-        <v>0.61162077818033744</v>
+        <v>0.94254264239140328</v>
       </c>
       <c r="E16">
-        <v>49644</v>
+        <v>517125.41369999998</v>
       </c>
       <c r="F16">
-        <v>1.049557183640409E-2</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>0.15513750000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.796789676554084E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -936,20 +876,16 @@
         <v>4539.9738461538454</v>
       </c>
       <c r="D17">
-        <v>0.11018818796440449</v>
+        <v>1.630139246494967E-2</v>
       </c>
       <c r="E17">
         <v>8943.7484769230759</v>
       </c>
       <c r="F17">
-        <v>1.89085800149617E-3</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>2.7949213990384612E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.1075701381704689E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -958,42 +894,34 @@
         <v>11462.02729411765</v>
       </c>
       <c r="D18">
-        <v>0.27819103385525812</v>
+        <v>4.1155965143647062E-2</v>
       </c>
       <c r="E18">
         <v>22580.193769411759</v>
       </c>
       <c r="F18">
-        <v>4.7738305895331824E-3</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>7.0563105529411752E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7.8456517480316422E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>41202.001140271488</v>
+        <v>278502.21114027151</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>81167.942246334831</v>
+        <v>548649.35594633489</v>
       </c>
       <c r="F19">
-        <v>1.716026042743345E-2</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>0.25364981951979637</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.9063218954161059E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1001,45 +929,37 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>7931000</v>
+        <v>82614649.424999997</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>95172</v>
+        <v>991375.79310000001</v>
       </c>
       <c r="F20">
-        <v>2.0120952437641011E-2</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>0.29741250000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.4446069433769502E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21">
-        <v>7931000</v>
+        <v>82614649.424999997</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>95172</v>
+        <v>991375.79310000001</v>
       </c>
       <c r="F21">
-        <v>2.0120952437641011E-2</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>0.29741250000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.4446069433769502E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -1047,23 +967,19 @@
         <v>16</v>
       </c>
       <c r="C22">
-        <v>83937.5</v>
+        <v>874349.65781250002</v>
       </c>
       <c r="D22">
-        <v>0.54776626662351835</v>
+        <v>0.92656322194893159</v>
       </c>
       <c r="E22">
-        <v>214040.625</v>
+        <v>2229591.627421875</v>
       </c>
       <c r="F22">
-        <v>4.5251767697935902E-2</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>0.66887695312499995</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7.7468774748848612E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
@@ -1072,42 +988,34 @@
         <v>69298.478764078478</v>
       </c>
       <c r="D23">
-        <v>0.45223373337648182</v>
+        <v>7.3436778051068408E-2</v>
       </c>
       <c r="E23">
         <v>176711.12084840011</v>
       </c>
       <c r="F23">
-        <v>3.7359686229068337E-2</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>0.55222225265125036</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6.1399557875317498E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C24">
-        <v>153235.97876407849</v>
+        <v>943648.13657657849</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>390751.74584840011</v>
+        <v>2406302.7482702751</v>
       </c>
       <c r="F24">
-        <v>8.2611453927004225E-2</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>1.2210992057762504</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8.3608730536380363E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1115,45 +1023,37 @@
         <v>16</v>
       </c>
       <c r="C25">
-        <v>475</v>
+        <v>4947.9206249999997</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>93575</v>
+        <v>974740.36312499992</v>
       </c>
       <c r="F25">
-        <v>1.9783319929729939E-2</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>0.292421875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.3868059379491673E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26">
-        <v>475</v>
+        <v>4947.9206249999997</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>93575</v>
+        <v>974740.36312499992</v>
       </c>
       <c r="F26">
-        <v>1.9783319929729939E-2</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>0.292421875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.3868059379491673E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1161,17 +1061,13 @@
         <v>22</v>
       </c>
       <c r="E27">
-        <v>4729994.7800660869</v>
+        <v>28780520.082447961</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>14.781233687706521</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1191,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1199,31 +1095,31 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>6912000.0000000075</v>
+        <v>4500003.6000000043</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>1340928.0000000009</v>
+        <v>873000.69840000081</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>6912000.0000000075</v>
+        <v>4500003.6000000043</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>1340928.0000000009</v>
+        <v>873000.69840000081</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1237,7 +1133,7 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <v>1340928.0000000009</v>
+        <v>873000.69840000081</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1262,13 +1158,13 @@
         <v>28</v>
       </c>
       <c r="B37">
-        <v>51410.19225198323</v>
+        <v>2940576.2546883812</v>
       </c>
       <c r="C37">
-        <v>1439485.38305553</v>
+        <v>82336135.131274655</v>
       </c>
       <c r="D37">
-        <v>-2.0209636484045621</v>
+        <v>1.3740568301280911</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1276,13 +1172,13 @@
         <v>29</v>
       </c>
       <c r="B38">
-        <v>62.690977811411891</v>
+        <v>653.03154129368886</v>
       </c>
       <c r="C38">
-        <v>16613.10912002415</v>
+        <v>173053.35844282751</v>
       </c>
       <c r="D38">
-        <v>-2.3323953138919731E-2</v>
+        <v>2.887980456768505E-3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1290,13 +1186,13 @@
         <v>30</v>
       </c>
       <c r="B39">
-        <v>173414.28104275971</v>
+        <v>1806400.205981089</v>
       </c>
       <c r="C39">
-        <v>-260121.42156413951</v>
+        <v>-2709600.3089716341</v>
       </c>
       <c r="D39">
-        <v>0.36519713457358882</v>
+        <v>-4.5218843531136983E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1304,13 +1200,13 @@
         <v>31</v>
       </c>
       <c r="B40">
-        <v>290357.06130187871</v>
+        <v>3024555.1415367471</v>
       </c>
       <c r="C40">
-        <v>-1567928.1310301451</v>
+        <v>-16332597.76429843</v>
       </c>
       <c r="D40">
-        <v>2.201290678892978</v>
+        <v>-0.27256462154785649</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1318,13 +1214,13 @@
         <v>32</v>
       </c>
       <c r="B41">
-        <v>30290.067027069701</v>
+        <v>315521.78394920123</v>
       </c>
       <c r="C41">
-        <v>-148421.32843264149</v>
+        <v>-1546056.7413510859</v>
       </c>
       <c r="D41">
-        <v>0.20837593277507549</v>
+        <v>-2.5801184641858609E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1332,13 +1228,13 @@
         <v>33</v>
       </c>
       <c r="B42">
-        <v>26441.304873984009</v>
+        <v>275430.4794482073</v>
       </c>
       <c r="C42">
-        <v>-39661.957310976009</v>
+        <v>-413145.71917231102</v>
       </c>
       <c r="D42">
-        <v>5.5683353852412083E-2</v>
+        <v>-6.8947333556741803E-3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1346,13 +1242,13 @@
         <v>34</v>
       </c>
       <c r="B43">
-        <v>11208.438521359159</v>
+        <v>116754.66133447889</v>
       </c>
       <c r="C43">
-        <v>-60525.568015339442</v>
+        <v>-630475.17120618594</v>
       </c>
       <c r="D43">
-        <v>8.4974793212832619E-2</v>
+        <v>-1.0521610151372989E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1360,13 +1256,13 @@
         <v>35</v>
       </c>
       <c r="B44">
-        <v>18717.717930912</v>
+        <v>194976.3844279827</v>
       </c>
       <c r="C44">
-        <v>-91716.817861468822</v>
+        <v>-955384.28369711549</v>
       </c>
       <c r="D44">
-        <v>0.12876570823659439</v>
+        <v>-1.5943817356960419E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1374,7 +1270,7 @@
         <v>15</v>
       </c>
       <c r="C45">
-        <v>-712276.73203915567</v>
+        <v>59921928.50102073</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1399,10 +1295,10 @@
         <v>37</v>
       </c>
       <c r="B49">
-        <v>457261.50416330918</v>
+        <v>456960</v>
       </c>
       <c r="C49">
-        <v>68589.225624496379</v>
+        <v>68544</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1413,7 +1309,7 @@
         <v>15</v>
       </c>
       <c r="C50">
-        <v>68589.225624496379</v>
+        <v>68544</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1421,16 +1317,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>